<commit_message>
updated test data sheet for tc_002
</commit_message>
<xml_diff>
--- a/jupiter-cloud/Data/tc_002.xlsx
+++ b/jupiter-cloud/Data/tc_002.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\installed\EclispseWorkspaces\jupiter-cloud\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SW\installed\EclispseWorkspaces\a\jupiter-cloud-prabhath\jupiter-cloud\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7142B357-C57E-4F94-8D70-B968FFDE2587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AEED7D-D0D2-41C2-A487-365B7E1956B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{002B31A8-901C-4AB6-8B7F-8F0812D7BFE4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>foreName</t>
   </si>
@@ -36,13 +36,49 @@
     <t>Message</t>
   </si>
   <si>
-    <t>Prabhath</t>
-  </si>
-  <si>
-    <t>prabath@gmail.com</t>
-  </si>
-  <si>
-    <t>TestMessage</t>
+    <t>Nice Service</t>
+  </si>
+  <si>
+    <t>Superb</t>
+  </si>
+  <si>
+    <t>So much appreciate your service</t>
+  </si>
+  <si>
+    <t>Excelent Support</t>
+  </si>
+  <si>
+    <t>Keep it up !</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Tony</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>tony@test.com.au</t>
+  </si>
+  <si>
+    <t>brian@test.com.au</t>
+  </si>
+  <si>
+    <t>james@test.com.au</t>
+  </si>
+  <si>
+    <t>john@test.com.au</t>
+  </si>
+  <si>
+    <t>smith@test.com.au</t>
   </si>
 </sst>
 </file>
@@ -405,17 +441,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A1DAC6-9910-4D7C-96D8-4795C3633EC8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -431,18 +467,66 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{37507E61-BDCD-4F55-8778-723C77FD0B2D}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{74F33E6B-A2DD-4499-9E3A-67B4BEA63B98}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{11221371-7093-453E-A1FB-4F26594CFF62}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{F8C9A81C-2BD9-4B5C-90EE-4BEC69D62860}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{2423A185-978E-449E-A9D7-CA2D9F03CCDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>